<commit_message>
manual connection - keyword for project type
</commit_message>
<xml_diff>
--- a/data/nlp/connections.xlsx
+++ b/data/nlp/connections.xlsx
@@ -1,27 +1,110 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20354"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Ptidej\wordcloud\ptidej-wordcloud\data\nlp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t_tuan\Documents\Research\2019\Wordcloud\ptidej-wordcloud\data\nlp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9E5C26E3-EF00-4FEC-AB77-C6ED32CFB2FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFB7348-99A3-4764-9664-612A6B152D8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="connection data" sheetId="1" r:id="rId1"/>
     <sheet name="manual connection" sheetId="3" r:id="rId2"/>
+    <sheet name="keywords" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tuan Tran</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{FB47C8CB-E4F9-4F45-8A85-0323B8AEA499}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tuan Tran:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+implementation of OPC UA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{7172604F-580D-4DD4-B180-A29F58CB2026}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tuan Tran:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+implement MQTT</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{596F44DD-4E8A-497C-8FB9-27CABB5FBA3C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tuan Tran:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Implement MQTT</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="135">
   <si>
     <t>paho</t>
   </si>
@@ -738,12 +821,27 @@
 volttron developer discussions
 volttron community discussions</t>
   </si>
+  <si>
+    <t>interchangable</t>
+  </si>
+  <si>
+    <t>can be used by</t>
+  </si>
+  <si>
+    <t>MQTT</t>
+  </si>
+  <si>
+    <t>OPC UA</t>
+  </si>
+  <si>
+    <t>OPC Unified Architecture</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,8 +976,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1077,6 +1188,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1238,7 +1355,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1247,6 +1364,9 @@
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1305,6 +1425,267 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Triangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B1A891B-6AD5-4FCD-BFC6-4A1E5CFEAB7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2190749" y="7991475"/>
+          <a:ext cx="2409825" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rtTriangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Right Triangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A039DB9-0C62-4C7C-8D42-EB9CC5597DC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="2209799" y="7924800"/>
+          <a:ext cx="2409825" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rtTriangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Arrow: Curved Up 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{154B794F-DAF2-4298-BFCA-CBDB1FB666BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1962149" y="8829675"/>
+          <a:ext cx="2676525" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedUpArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 25000"/>
+            <a:gd name="adj2" fmla="val 51381"/>
+            <a:gd name="adj3" fmla="val 25000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Arrow: Curved Up 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5C2AFF7-0E90-41B2-8563-9AC2192FFA65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="2219324" y="7181850"/>
+          <a:ext cx="2676525" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedUpArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 25000"/>
+            <a:gd name="adj2" fmla="val 51381"/>
+            <a:gd name="adj3" fmla="val 25000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1603,7 +1984,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2453,19 +2834,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AL38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -2587,8 +2970,8 @@
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
+      <c r="E2" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>37</v>
@@ -2655,6 +3038,14 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5" s="2"/>
       <c r="G5" s="5" t="s">
         <v>49</v>
       </c>
@@ -3294,6 +3685,37 @@
         <v>35</v>
       </c>
       <c r="AL38" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51731D49-8734-4F7D-9344-C674E5AAF704}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update keywords for projects
</commit_message>
<xml_diff>
--- a/data/nlp/connections.xlsx
+++ b/data/nlp/connections.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20354"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t_tuan\Documents\Research\2019\Wordcloud\ptidej-wordcloud\data\nlp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88229256-4995-4E73-94B6-ECA0A41BB300}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B176EEB-583E-475A-9054-912C9D8AA4CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
   <si>
     <t>paho</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>Eclipse fog05</t>
-  </si>
-  <si>
-    <t>"./lwm2mclient -4 -h leshan.eclipse.org"</t>
   </si>
   <si>
     <t>A more charming argument for software update is that it enables agile development for hardware and hardware near development.</t>
@@ -291,6 +288,35 @@
   </si>
   <si>
     <t>digital twin</t>
+  </si>
+  <si>
+    <t>Implement LWM2M (Lightweight M2M)
+Using CoAP</t>
+  </si>
+  <si>
+    <t>Using OSGi</t>
+  </si>
+  <si>
+    <t>Implement oneM2M and smartM2M</t>
+  </si>
+  <si>
+    <t>Using MQTT
+Using AMQT
+Support MQTT
+Support HTTP
+Suport CoAP</t>
+  </si>
+  <si>
+    <t>Conform with SCADA architecture</t>
+  </si>
+  <si>
+    <t>Implement OSGi</t>
+  </si>
+  <si>
+    <t>language and interface for digital twin</t>
+  </si>
+  <si>
+    <t>using IEC 61499 standard</t>
   </si>
 </sst>
 </file>
@@ -441,7 +467,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -636,6 +662,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,7 +833,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -812,6 +844,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1363,15 +1400,19 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
@@ -1418,7 +1459,7 @@
       <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -1490,52 +1531,52 @@
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
       <c r="F3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" t="s">
         <v>45</v>
       </c>
-      <c r="S3" t="s">
+      <c r="AA3" t="s">
         <v>46</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AG3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2"/>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
     </row>
     <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
@@ -1544,20 +1585,20 @@
       <c r="F5" s="1"/>
       <c r="K5" s="1"/>
       <c r="S5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
     </row>
     <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2"/>
       <c r="H6" s="1"/>
@@ -1565,13 +1606,13 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="M6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1592,7 +1633,7 @@
     </row>
     <row r="7" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -1601,38 +1642,41 @@
     </row>
     <row r="8" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="2"/>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K8" s="1"/>
       <c r="R8" t="s">
+        <v>53</v>
+      </c>
+      <c r="U8" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="U8" s="5" t="s">
+      <c r="AG8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AH8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AH8" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="AI8" s="1"/>
     </row>
-    <row r="9" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="2"/>
       <c r="K9" s="1"/>
-      <c r="P9" t="s">
-        <v>37</v>
+      <c r="P9" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="AH9" s="1"/>
     </row>
@@ -1643,16 +1687,19 @@
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
       <c r="Z10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AD10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AH10" s="1" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1679,31 +1726,40 @@
       <c r="AL11" s="1"/>
     </row>
     <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L12" s="2"/>
       <c r="P12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T12" t="s">
         <v>17</v>
       </c>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AI12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1712,40 +1768,54 @@
       <c r="AH14" s="1"/>
     </row>
     <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="O15" s="2"/>
       <c r="AH15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="I16" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="P16" s="2"/>
     </row>
-    <row r="17" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+    <row r="17" spans="1:38" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q17" s="2"/>
-      <c r="AI17" s="1"/>
-    </row>
-    <row r="18" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI17" s="8"/>
+    </row>
+    <row r="18" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="R18" s="2"/>
       <c r="AG18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AH18" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1754,19 +1824,19 @@
         <v>17</v>
       </c>
       <c r="AA19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AG19" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AH19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AI19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1774,17 +1844,17 @@
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
     </row>
-    <row r="21" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="U21" s="2"/>
       <c r="Y21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH21" s="1"/>
     </row>
-    <row r="22" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
@@ -1792,7 +1862,7 @@
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
     </row>
-    <row r="23" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
@@ -1800,63 +1870,63 @@
       <c r="AH23" s="1"/>
       <c r="AI23" s="1"/>
     </row>
-    <row r="24" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="X24" s="2"/>
       <c r="AG24" s="1"/>
       <c r="AH24" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="Y25" s="2"/>
       <c r="AH25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AI25" s="1"/>
     </row>
-    <row r="26" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="Z26" s="2"/>
       <c r="AH26" s="1"/>
     </row>
-    <row r="27" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="AA27" s="2"/>
       <c r="AH27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI27" s="1"/>
       <c r="AL27" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="AB28" s="2"/>
       <c r="AH28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AI28" s="1"/>
     </row>
-    <row r="29" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="AC29" s="2"/>
     </row>
-    <row r="30" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
@@ -1864,7 +1934,7 @@
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
     </row>
-    <row r="31" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
@@ -1872,7 +1942,7 @@
       <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
     </row>
-    <row r="32" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>28</v>
       </c>
@@ -1886,10 +1956,10 @@
       </c>
       <c r="AG33" s="2"/>
       <c r="AH33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI33" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="AI33" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1958,15 +2028,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish manual analysis of projects
</commit_message>
<xml_diff>
--- a/data/nlp/connections.xlsx
+++ b/data/nlp/connections.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t_tuan\Documents\Research\2019\Wordcloud\ptidej-wordcloud\data\nlp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Ptidej\wordcloud\ptidej-wordcloud\data\nlp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31519577-C367-455E-82ED-7C4205FE5B51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5827581C-852D-4699-B049-A75BB7E2B002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,6 +24,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tuan Tran</author>
+    <author>tc={3FF0303F-A426-4988-B78B-3F6F4CBEAEC9}</author>
   </authors>
   <commentList>
     <comment ref="A28" authorId="0" shapeId="0" xr:uid="{320E9C11-2CCA-4F24-BFD2-A412282E2186}">
@@ -75,12 +76,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="B37" authorId="1" shapeId="0" xr:uid="{3FF0303F-A426-4988-B78B-3F6F4CBEAEC9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    no source code, developer contact available</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="130">
   <si>
     <t>paho</t>
   </si>
@@ -495,6 +504,28 @@
   </si>
   <si>
     <t>implement Sparkplug (a specification of MQTT)</t>
+  </si>
+  <si>
+    <t>support ZeroMQ (ZMQ)
+Support RabbitMQ</t>
+  </si>
+  <si>
+    <t>ZMQ</t>
+  </si>
+  <si>
+    <t>ZeroMQ</t>
+  </si>
+  <si>
+    <t>RabbitMQ</t>
+  </si>
+  <si>
+    <t>Using Calypso standard</t>
+  </si>
+  <si>
+    <t>Calypso</t>
+  </si>
+  <si>
+    <t>the standard for contactless tickets and cards</t>
   </si>
 </sst>
 </file>
@@ -1315,6 +1346,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Tuan Tran" id="{368444AF-E8CE-4161-BDD8-BE33586D40E4}" userId="b3f017eb7601ac85" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1610,6 +1647,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B37" dT="2020-04-04T20:28:46.11" personId="{368444AF-E8CE-4161-BDD8-BE33586D40E4}" id="{3FF0303F-A426-4988-B78B-3F6F4CBEAEC9}">
+    <text>no source code, developer contact available</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL37"/>
@@ -1618,7 +1663,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,6 +1682,7 @@
     <col min="21" max="21" width="16.5703125" customWidth="1"/>
     <col min="28" max="28" width="9.140625" style="7"/>
     <col min="33" max="33" width="9.140625" style="7"/>
+    <col min="38" max="38" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -1746,7 +1792,7 @@
       <c r="AK1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2244,7 +2290,7 @@
       <c r="AI33" s="1"/>
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
-      <c r="AL33" s="1"/>
+      <c r="AL33" s="8"/>
     </row>
     <row r="34" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -2255,23 +2301,28 @@
       </c>
       <c r="AI34" s="2"/>
     </row>
-    <row r="35" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="B35" s="3" t="s">
         <v>33</v>
       </c>
       <c r="AJ35" s="2"/>
     </row>
     <row r="36" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>127</v>
+      </c>
       <c r="B36" s="3" t="s">
         <v>34</v>
       </c>
       <c r="AK36" s="2"/>
     </row>
-    <row r="37" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+    <row r="37" spans="1:38" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AL37" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2287,10 +2338,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51731D49-8734-4F7D-9344-C674E5AAF704}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2398,6 +2449,27 @@
         <v>116</v>
       </c>
     </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
table of protocols, table of keywords
</commit_message>
<xml_diff>
--- a/data/nlp/connections.xlsx
+++ b/data/nlp/connections.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Ptidej\wordcloud\ptidej-wordcloud\data\nlp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5827581C-852D-4699-B049-A75BB7E2B002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D35DFD-BDF0-4234-BE93-0741709355BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="connection data" sheetId="1" r:id="rId1"/>
     <sheet name="keywords" sheetId="4" r:id="rId2"/>
+    <sheet name="Others" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -89,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="137">
   <si>
     <t>paho</t>
   </si>
@@ -219,9 +220,6 @@
   </si>
   <si>
     <t>OPC UA</t>
-  </si>
-  <si>
-    <t>OPC Unified Architecture</t>
   </si>
   <si>
     <t>paho.incubator-dev
@@ -448,9 +446,6 @@
     <t>ABAC</t>
   </si>
   <si>
-    <t>Attribute Based Access Control</t>
-  </si>
-  <si>
     <t>this is a process (like agile)</t>
   </si>
   <si>
@@ -526,6 +521,33 @@
   </si>
   <si>
     <t>the standard for contactless tickets and cards</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Meanings</t>
+  </si>
+  <si>
+    <t>Message Queuing Telemetry Transport</t>
+  </si>
+  <si>
+    <t>Is Protocol</t>
+  </si>
+  <si>
+    <t>Open Platform Communication Unified Architecture</t>
+  </si>
+  <si>
+    <t>Attribute-based access control</t>
+  </si>
+  <si>
+    <t>Is Abstract</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>open-source message-broker software</t>
   </si>
 </sst>
 </file>
@@ -1659,7 +1681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1798,7 +1820,7 @@
     </row>
     <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1809,41 +1831,41 @@
       </c>
       <c r="K2" s="1"/>
       <c r="Q2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" t="s">
         <v>44</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AA2" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AF2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="AG2" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2"/>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="8"/>
     </row>
     <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
@@ -1852,14 +1874,14 @@
       <c r="F4" s="1"/>
       <c r="K4" s="1"/>
       <c r="S4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AG4" s="8"/>
       <c r="AH4" s="1"/>
     </row>
     <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
@@ -1873,13 +1895,13 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="M5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1900,7 +1922,7 @@
     </row>
     <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -1909,33 +1931,33 @@
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="2"/>
       <c r="J7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K7" s="1"/>
       <c r="R7" t="s">
+        <v>52</v>
+      </c>
+      <c r="U7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="AF7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AG7" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="AG7" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="AH7" s="1"/>
     </row>
     <row r="8" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
@@ -1957,15 +1979,15 @@
         <v>37</v>
       </c>
       <c r="AC9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG9" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AG9" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -1994,7 +2016,7 @@
     </row>
     <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
@@ -2008,7 +2030,7 @@
       </c>
       <c r="AF11" s="1"/>
       <c r="AG11" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH11" t="s">
         <v>36</v>
@@ -2016,7 +2038,7 @@
     </row>
     <row r="12" spans="1:38" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>10</v>
@@ -2028,7 +2050,7 @@
     </row>
     <row r="13" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
@@ -2039,19 +2061,19 @@
     </row>
     <row r="14" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="O14" s="2"/>
       <c r="AG14" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:38" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>13</v>
@@ -2069,22 +2091,22 @@
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="R17" s="2"/>
       <c r="AF17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG17" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="AG17" s="8" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>16</v>
@@ -2094,13 +2116,13 @@
         <v>17</v>
       </c>
       <c r="AA18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AF18" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="AG18" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH18" t="s">
         <v>36</v>
@@ -2108,7 +2130,7 @@
     </row>
     <row r="19" spans="1:37" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>17</v>
@@ -2119,7 +2141,7 @@
     </row>
     <row r="20" spans="1:37" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>18</v>
@@ -2135,13 +2157,13 @@
     </row>
     <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V21" s="2"/>
       <c r="AF21" s="1"/>
@@ -2157,36 +2179,36 @@
     </row>
     <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U23" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X23" s="2"/>
       <c r="AF23" s="1"/>
       <c r="AG23" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="Y24" s="2"/>
       <c r="AG24" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AH24" s="1"/>
     </row>
@@ -2199,35 +2221,35 @@
     </row>
     <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
       <c r="AA26" s="2"/>
       <c r="AG26" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AH26" s="1"/>
       <c r="AK26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:37" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>25</v>
       </c>
       <c r="AG27" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AH27" s="8"/>
     </row>
     <row r="28" spans="1:37" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>26</v>
@@ -2238,7 +2260,7 @@
     </row>
     <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>27</v>
@@ -2249,7 +2271,7 @@
     </row>
     <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>28</v>
@@ -2260,17 +2282,17 @@
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
       <c r="AF31" s="2"/>
       <c r="AG31" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH31" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="AH31" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:37" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2294,7 +2316,7 @@
     </row>
     <row r="34" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>32</v>
@@ -2303,7 +2325,7 @@
     </row>
     <row r="35" spans="1:38" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>33</v>
@@ -2312,7 +2334,7 @@
     </row>
     <row r="36" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>34</v>
@@ -2338,140 +2360,224 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51731D49-8734-4F7D-9344-C674E5AAF704}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="67" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="I1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" t="s">
-        <v>97</v>
-      </c>
-      <c r="O2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" t="s">
         <v>85</v>
       </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" t="s">
-        <v>98</v>
-      </c>
-      <c r="O3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" t="s">
         <v>92</v>
       </c>
-      <c r="B4" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>104</v>
       </c>
-      <c r="I5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>107</v>
       </c>
-      <c r="I6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>110</v>
       </c>
-      <c r="I7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
       <c r="B10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12" t="s">
-        <v>129</v>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E19945-9A98-4771-B771-37415F7DB15A}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change from default pos_tag to standford pos_tag
</commit_message>
<xml_diff>
--- a/data/nlp/connections.xlsx
+++ b/data/nlp/connections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Ptidej\wordcloud\ptidej-wordcloud\data\nlp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83AD614-8049-4728-BCDF-9645ADF36318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4DF008-AD97-4307-ACC1-941CCFC93BF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="195">
   <si>
     <t>paho</t>
   </si>
@@ -575,18 +575,12 @@
     <t>Connect IoT devices to Kapua via MQTT</t>
   </si>
   <si>
-    <t>apply MQTT</t>
-  </si>
-  <si>
     <t>Noun</t>
   </si>
   <si>
     <t>NN</t>
   </si>
   <si>
-    <t>noun, singular (cat, tree)</t>
-  </si>
-  <si>
     <t>NNS</t>
   </si>
   <si>
@@ -656,9 +650,6 @@
     <t>through</t>
   </si>
   <si>
-    <t>noun, plural (desks)</t>
-  </si>
-  <si>
     <t>protocol</t>
   </si>
   <si>
@@ -666,6 +657,72 @@
   </si>
   <si>
     <t>Relationship</t>
+  </si>
+  <si>
+    <t>VBG</t>
+  </si>
+  <si>
+    <t>Verb</t>
+  </si>
+  <si>
+    <t>verb, gerund/present participle</t>
+  </si>
+  <si>
+    <t>using</t>
+  </si>
+  <si>
+    <t>communicating</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>any words</t>
+  </si>
+  <si>
+    <t>Adjective</t>
+  </si>
+  <si>
+    <t>noun plural</t>
+  </si>
+  <si>
+    <t>noun singular</t>
+  </si>
+  <si>
+    <t>protocols</t>
+  </si>
+  <si>
+    <t>any, via, common</t>
+  </si>
+  <si>
+    <t>applying MQTT</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>sent over different protocols (REST, MQTT, AMQP)</t>
+  </si>
+  <si>
+    <t>apply</t>
+  </si>
+  <si>
+    <t>VB</t>
+  </si>
+  <si>
+    <t>verb base form</t>
+  </si>
+  <si>
+    <t>connect</t>
+  </si>
+  <si>
+    <t>sent</t>
+  </si>
+  <si>
+    <t>via</t>
+  </si>
+  <si>
+    <t>over</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1195,6 +1252,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1241,7 +1335,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1264,9 +1358,6 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1275,9 +1366,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1294,8 +1382,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2761,10 +2898,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEF6D51-A789-480E-B850-E705BE67357B}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2773,7 +2910,7 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" customWidth="1"/>
@@ -2785,303 +2922,688 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="A1" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
       <c r="M1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="E2" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+      <c r="A3" s="22">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>158</v>
+      <c r="D3" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>156</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="11"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>159</v>
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>157</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="34"/>
       <c r="M4" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
       <c r="M5" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="15" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="M6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="M6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15" t="s">
-        <v>162</v>
-      </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="20" t="s">
-        <v>168</v>
+      <c r="G7" s="18" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="D8" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
       <c r="M8" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="17" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
       <c r="M9" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="17" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+      <c r="A11" s="22">
         <v>2</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="28"/>
+      <c r="M11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F12" s="34"/>
+      <c r="G12" s="29"/>
+      <c r="M12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="24" t="s">
+      <c r="D13" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="M13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="M15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>170</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>173</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="24" t="s">
-        <v>174</v>
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="21" t="s">
+        <v>171</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="16"/>
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="22">
+        <v>3</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="35"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O20" t="s">
-        <v>141</v>
-      </c>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="29"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O21" t="s">
-        <v>142</v>
+      <c r="A21" s="22"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="21" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O22" t="s">
-        <v>143</v>
-      </c>
+      <c r="A22" s="22"/>
+      <c r="B22" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O23" t="s">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="O24" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O24" t="s">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="O25" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="22">
+        <v>4</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="11" t="s">
         <v>145</v>
       </c>
+      <c r="C31" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" s="36"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="28">
+        <v>5</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="33"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="35"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" s="34"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="35"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="35"/>
+      <c r="B35" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="35"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="35"/>
+      <c r="B38" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="35"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="29"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="63">
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="A32:A40"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="C13:C15"/>
@@ -3098,9 +3620,6 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>